<commit_message>
editing the Gant Chart
</commit_message>
<xml_diff>
--- a/docs/GantChart_Azelele_MGuz.xlsx
+++ b/docs/GantChart_Azelele_MGuz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\Downloads\Spring 2025\CS-230\Final Project Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\FinalProject\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E7AA991-C5A5-47D8-A961-0B860EB1A81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED5C28F-0E3F-43A8-8FA0-6207106E27EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
   </bookViews>
@@ -1135,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF3DB2-1A6B-144B-8344-5E254C7EE240}">
   <dimension ref="A1:DX47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="52" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="52" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -8553,7 +8553,7 @@
         <v/>
       </c>
       <c r="DQ18" s="7" t="str">
-        <f t="shared" ref="DQ18:DZ24" si="36">IF(DQ$4=$F19,"u","")</f>
+        <f t="shared" ref="DQ18:DX24" si="36">IF(DQ$4=$F19,"u","")</f>
         <v/>
       </c>
       <c r="DR18" s="7" t="str">
@@ -11944,7 +11944,7 @@
         <v/>
       </c>
       <c r="CN25" s="7" t="str">
-        <f t="shared" ref="CN25:CW27" si="47">IF(CN$4=$F26,"u","")</f>
+        <f t="shared" ref="CN25:CN27" si="47">IF(CN$4=$F26,"u","")</f>
         <v/>
       </c>
       <c r="CO25" s="7" t="str">
@@ -12068,7 +12068,7 @@
         <v/>
       </c>
       <c r="DS25" s="7" t="str">
-        <f t="shared" ref="DS25:EB28" si="51">IF(DS$4=$F24,"u","")</f>
+        <f t="shared" ref="DS25:DX28" si="51">IF(DS$4=$F24,"u","")</f>
         <v/>
       </c>
       <c r="DT25" s="7" t="str">

</xml_diff>

<commit_message>
editied the giannt chart
</commit_message>
<xml_diff>
--- a/docs/GantChart_Azelele_MGuz.xlsx
+++ b/docs/GantChart_Azelele_MGuz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\FinalProject\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED5C28F-0E3F-43A8-8FA0-6207106E27EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906D5B00-38DC-46E0-9126-C7F8E1DC2DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
   </bookViews>
@@ -1135,15 +1135,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF3DB2-1A6B-144B-8344-5E254C7EE240}">
   <dimension ref="A1:DX47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="52" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="52" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="51.83203125" customWidth="1"/>
+    <col min="3" max="3" width="57.4140625" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="17.9140625" customWidth="1"/>
@@ -3099,7 +3099,7 @@
         <v>13</v>
       </c>
       <c r="I8" s="32">
-        <v>0.6</v>
+        <v>0.63</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="7" t="str">
@@ -4101,7 +4101,7 @@
         <v>13</v>
       </c>
       <c r="I10" s="32">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="7" t="str">
@@ -5604,7 +5604,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="32">
-        <v>0.65</v>
+        <v>1</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="7" t="str">
@@ -6606,7 +6606,7 @@
         <v>12</v>
       </c>
       <c r="I15" s="32">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="7" t="str">

</xml_diff>

<commit_message>
edited the flow chart
</commit_message>
<xml_diff>
--- a/docs/GantChart_Azelele_MGuz.xlsx
+++ b/docs/GantChart_Azelele_MGuz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muratguzelocak/Documents/Projects/FreeBomber/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\FinalProject\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69080DA5-4639-2C44-9668-8C4D974D6696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCF7AE0-B43F-4C4E-8598-C84601991D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="30620" windowHeight="17040" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
   <si>
     <t>Project Start Date:</t>
   </si>
@@ -110,25 +110,10 @@
     <t>2 Enemy Character Dev</t>
   </si>
   <si>
-    <t>Player Login GUI</t>
-  </si>
-  <si>
-    <t>Player Info Storage</t>
-  </si>
-  <si>
-    <t>Score Keeper Dev</t>
-  </si>
-  <si>
-    <t>Testing and Validation</t>
-  </si>
-  <si>
     <t>Collision Detection Dev</t>
   </si>
   <si>
     <t>Vision Statement Write-Up</t>
-  </si>
-  <si>
-    <t>Bomb Development</t>
   </si>
   <si>
     <t>Champ. Player Special Abilities Dev</t>
@@ -140,28 +125,31 @@
     <t>2 Enemy's Special Abilities Dev</t>
   </si>
   <si>
-    <t>The Special Door Dev</t>
-  </si>
-  <si>
     <t>Creating 5 Levels(Maps)</t>
-  </si>
-  <si>
-    <t>Level-Up Dev</t>
   </si>
   <si>
     <t>Merging and Status Update Meeting</t>
   </si>
   <si>
-    <t>Champ. Player Health Dev</t>
+    <t>Game Background Setup</t>
   </si>
   <si>
-    <t>Game Timer Dev</t>
+    <t>Bomb animation</t>
   </si>
   <si>
-    <t>Game Manual</t>
+    <t>Bomb destruction</t>
   </si>
   <si>
-    <t>Game Background Setup</t>
+    <t>Comment Background and Tile Manager Class</t>
+  </si>
+  <si>
+    <t>Special door Dev</t>
+  </si>
+  <si>
+    <t>Comment all Enemy Classes</t>
+  </si>
+  <si>
+    <t>Comment Character and JackBomber Classes</t>
   </si>
 </sst>
 </file>
@@ -174,7 +162,7 @@
     <numFmt numFmtId="166" formatCode="mmm\-d\-yy"/>
     <numFmt numFmtId="167" formatCode="mmm\-d"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -550,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
@@ -660,143 +648,12 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EF8FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB2C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EF8FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB2C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EF8FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB2C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="9"/>
-        </left>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF9EF8FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFDBFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB2C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC7F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -1238,11 +1095,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF3DB2-1A6B-144B-8344-5E254C7EE240}">
   <dimension ref="A1:DX47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
@@ -1267,8 +1124,8 @@
     <col min="77" max="77" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:128" ht="54" customHeight="1" thickBot="1"/>
-    <row r="2" spans="1:128" ht="25" thickBot="1">
+    <row r="1" spans="1:128" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:128" ht="24" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -1403,7 +1260,7 @@
       <c r="DW2" s="38"/>
       <c r="DX2" s="39"/>
     </row>
-    <row r="3" spans="1:128" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
+    <row r="3" spans="1:128" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3"/>
       <c r="B3" s="15"/>
       <c r="C3" s="33" t="s">
@@ -1549,7 +1406,7 @@
       <c r="DW3" s="35"/>
       <c r="DX3" s="36"/>
     </row>
-    <row r="4" spans="1:128" s="1" customFormat="1" ht="41" customHeight="1">
+    <row r="4" spans="1:128" s="1" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4"/>
       <c r="B4" s="18"/>
       <c r="C4" s="19" t="s">
@@ -2039,7 +1896,7 @@
         <v>45813</v>
       </c>
     </row>
-    <row r="5" spans="1:128" ht="23">
+    <row r="5" spans="1:128" ht="25.5" x14ac:dyDescent="0.4">
       <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
@@ -2184,7 +2041,7 @@
       <c r="DW5" s="4"/>
       <c r="DX5" s="11"/>
     </row>
-    <row r="6" spans="1:128" ht="27" customHeight="1">
+    <row r="6" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="23">
         <v>1</v>
       </c>
@@ -2683,13 +2540,13 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:128" ht="27" customHeight="1">
+    <row r="7" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="23">
         <f>B6+1</f>
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>16</v>
@@ -3184,7 +3041,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:128" ht="27" customHeight="1">
+    <row r="8" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="23">
         <f t="shared" ref="B8:B38" si="6">B7+1</f>
         <v>3</v>
@@ -3209,7 +3066,7 @@
         <v>13</v>
       </c>
       <c r="I8" s="32">
-        <v>0.63</v>
+        <v>0.65</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="7" t="str">
@@ -3685,7 +3542,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:128" ht="27" customHeight="1">
+    <row r="9" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="23">
         <f t="shared" si="6"/>
         <v>4</v>
@@ -4186,7 +4043,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:128" ht="27" customHeight="1">
+    <row r="10" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="23">
         <f t="shared" si="6"/>
         <v>5</v>
@@ -4201,11 +4058,11 @@
         <v>45716</v>
       </c>
       <c r="F10" s="30">
-        <v>45721</v>
+        <v>45737</v>
       </c>
       <c r="G10" s="27">
         <f t="shared" ref="G10" si="8">IF(F10="","",NETWORKDAYS(E10,F10))</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="H10" s="31" t="s">
         <v>13</v>
@@ -4316,71 +4173,71 @@
       </c>
       <c r="AJ10" s="7" t="str">
         <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AK10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AL10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AM10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AN10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AO10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AP10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AQ10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AR10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AS10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AT10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AU10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AV10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AW10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AX10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AY10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="AZ10" s="7" t="str">
+        <f t="shared" si="7"/>
         <v>u</v>
-      </c>
-      <c r="AK10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AL10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AM10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AN10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AO10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AP10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AQ10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AR10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AS10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AT10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AU10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AV10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AW10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AX10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AY10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AZ10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
       </c>
       <c r="BA10" s="7" t="str">
         <f t="shared" si="7"/>
@@ -4687,13 +4544,13 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:128" ht="27" customHeight="1">
+    <row r="11" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="23">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>16</v>
@@ -5188,13 +5045,13 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:128" ht="27" customHeight="1">
+    <row r="12" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="23">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>16</v>
@@ -5689,13 +5546,13 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:128" ht="27" customHeight="1">
+    <row r="13" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="23">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>16</v>
@@ -5711,7 +5568,7 @@
         <v>8</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I13" s="32">
         <v>1</v>
@@ -6190,7 +6047,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:128" ht="27" customHeight="1">
+    <row r="14" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="23">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -6691,7 +6548,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:128" ht="27" customHeight="1">
+    <row r="15" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="23">
         <f t="shared" si="6"/>
         <v>10</v>
@@ -6713,10 +6570,10 @@
         <v>5</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I15" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="7" t="str">
@@ -7192,13 +7049,13 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:128" ht="27" customHeight="1">
+    <row r="16" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="23">
         <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>19</v>
@@ -7214,7 +7071,7 @@
         <v>6</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I16" s="32">
         <v>0.5</v>
@@ -7693,22 +7550,22 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:128" ht="27" customHeight="1">
+    <row r="17" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="23">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="30">
-        <v>45726</v>
+        <v>45737</v>
       </c>
       <c r="F17" s="30">
-        <v>45733</v>
+        <v>45744</v>
       </c>
       <c r="G17" s="27">
         <f>IF(F17="","",NETWORKDAYS(E17,F17))</f>
@@ -7871,51 +7728,51 @@
       </c>
       <c r="AV17" s="7" t="str">
         <f>IF(AV$4=$F17,"u","")</f>
+        <v/>
+      </c>
+      <c r="AW17" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AX17" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AY17" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AZ17" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BA17" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BB17" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BC17" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BD17" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BE17" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BF17" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BG17" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>u</v>
-      </c>
-      <c r="AW17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AX17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AY17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AZ17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BA17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BB17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BC17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BD17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BE17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BF17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BG17" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
       </c>
       <c r="BH17" s="7" t="str">
         <f t="shared" si="21"/>
@@ -8194,13 +8051,13 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:128" ht="27" customHeight="1">
+    <row r="18" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="23">
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>16</v>
@@ -8209,17 +8066,17 @@
         <v>45723</v>
       </c>
       <c r="F18" s="30">
-        <v>45729</v>
+        <v>45737</v>
       </c>
       <c r="G18" s="27">
         <f t="shared" ref="G18" si="24">IF(F18="","",NETWORKDAYS(E18,F18))</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I18" s="32">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="7" t="str">
@@ -8356,40 +8213,40 @@
       </c>
       <c r="AR18" s="7" t="str">
         <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AS18" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AT18" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AU18" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AV18" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AW18" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AX18" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AY18" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AZ18" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>u</v>
       </c>
-      <c r="AS18" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AT18" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AU18" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AV18" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AW18" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AX18" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AY18" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AZ18" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
       <c r="BA18" s="7" t="str">
         <f t="shared" si="21"/>
         <v/>
@@ -8695,13 +8552,13 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:128" ht="27" customHeight="1">
+    <row r="19" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="23">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>19</v>
@@ -8710,17 +8567,17 @@
         <v>45723</v>
       </c>
       <c r="F19" s="30">
-        <v>45729</v>
+        <v>45737</v>
       </c>
       <c r="G19" s="27">
-        <f t="shared" ref="G19:G29" si="25">IF(F19="","",NETWORKDAYS(E19,F19))</f>
-        <v>5</v>
+        <f t="shared" ref="G19:G20" si="25">IF(F19="","",NETWORKDAYS(E19,F19))</f>
+        <v>11</v>
       </c>
       <c r="H19" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I19" s="32">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="7" t="str">
@@ -8857,45 +8714,45 @@
       </c>
       <c r="AR19" s="7" t="str">
         <f>IF(AR$4=$F19,"u","")</f>
+        <v/>
+      </c>
+      <c r="AS19" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AT19" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AU19" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AV19" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AW19" s="7" t="str">
+        <f>IF(AW$4=$F19,"u","")</f>
+        <v/>
+      </c>
+      <c r="AX19" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AY19" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="AZ19" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>u</v>
       </c>
-      <c r="AS19" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AT19" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AU19" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AV19" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AW19" s="43" t="str">
-        <f>IF(AW$4=$F19,"u","")</f>
-        <v/>
-      </c>
-      <c r="AX19" s="43" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AY19" s="43" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="AZ19" s="43" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BA19" s="43" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BB19" s="43" t="str">
+      <c r="BA19" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BB19" s="7" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -9196,26 +9053,26 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:128" ht="27" customHeight="1">
+    <row r="20" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="23">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E20" s="30">
-        <v>45734</v>
+        <v>45744</v>
       </c>
       <c r="F20" s="30">
-        <v>45738</v>
+        <v>45751</v>
       </c>
       <c r="G20" s="27">
         <f t="shared" si="25"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H20" s="31" t="s">
         <v>12</v>
@@ -9394,7 +9251,7 @@
       </c>
       <c r="BA20" s="7" t="str">
         <f>IF(BA$4=$F20,"u","")</f>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BB20" s="7" t="str">
         <f t="shared" si="21"/>
@@ -9446,7 +9303,7 @@
       </c>
       <c r="BN20" s="7" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BO20" s="7" t="str">
         <f t="shared" si="21"/>
@@ -9697,16 +9554,16 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:128" ht="27" customHeight="1">
+    <row r="21" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="23">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E21" s="30">
         <v>45740</v>
@@ -9715,7 +9572,7 @@
         <v>45740</v>
       </c>
       <c r="G21" s="27">
-        <f t="shared" si="25"/>
+        <f>IF(F21="","",NETWORKDAYS(E21,F21))</f>
         <v>1</v>
       </c>
       <c r="H21" s="31" t="s">
@@ -10198,29 +10055,29 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:128" ht="27" customHeight="1">
+    <row r="22" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="23">
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D22" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="30">
-        <v>45717</v>
+        <v>45733</v>
       </c>
       <c r="F22" s="30">
-        <v>45762</v>
+        <v>45737</v>
       </c>
       <c r="G22" s="27">
-        <f t="shared" si="25"/>
-        <v>32</v>
+        <f>IF(F22="","",NETWORKDAYS(E22,F22))</f>
+        <v>5</v>
       </c>
       <c r="H22" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I22" s="32">
         <v>0</v>
@@ -10392,7 +10249,7 @@
       </c>
       <c r="AZ22" s="7" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BA22" s="7" t="str">
         <f t="shared" si="21"/>
@@ -10492,7 +10349,7 @@
       </c>
       <c r="BY22" s="7" t="str">
         <f t="shared" si="22"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ22" s="7" t="str">
         <f t="shared" si="22"/>
@@ -10699,26 +10556,26 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:128" ht="27" customHeight="1">
+    <row r="23" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="23">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E23" s="30">
-        <v>45717</v>
+        <v>45737</v>
       </c>
       <c r="F23" s="30">
-        <v>45762</v>
+        <v>45744</v>
       </c>
       <c r="G23" s="27">
-        <f t="shared" si="25"/>
-        <v>32</v>
+        <f>IF(F23="","",NETWORKDAYS(E23,F23))</f>
+        <v>6</v>
       </c>
       <c r="H23" s="31" t="s">
         <v>12</v>
@@ -10921,7 +10778,7 @@
       </c>
       <c r="BG23" s="7" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BH23" s="7" t="str">
         <f t="shared" si="21"/>
@@ -10993,7 +10850,7 @@
       </c>
       <c r="BY23" s="7" t="str">
         <f t="shared" si="22"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ23" s="7" t="str">
         <f t="shared" si="22"/>
@@ -11200,26 +11057,26 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:128" ht="27" customHeight="1">
+    <row r="24" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="23">
         <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E24" s="30">
-        <v>45717</v>
+        <v>45737</v>
       </c>
       <c r="F24" s="30">
-        <v>45762</v>
+        <v>45744</v>
       </c>
       <c r="G24" s="27">
-        <f t="shared" si="25"/>
-        <v>32</v>
+        <f>IF(F24="","",NETWORKDAYS(E24,F24))</f>
+        <v>6</v>
       </c>
       <c r="H24" s="31" t="s">
         <v>12</v>
@@ -11353,7 +11210,7 @@
         <v/>
       </c>
       <c r="AP24" s="7" t="str">
-        <f t="shared" ref="K24:AP38" si="26">IF(AP$4=$F24,"u","")</f>
+        <f t="shared" ref="K24:AP32" si="26">IF(AP$4=$F24,"u","")</f>
         <v/>
       </c>
       <c r="AQ24" s="7" t="str">
@@ -11422,7 +11279,7 @@
       </c>
       <c r="BG24" s="7" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BH24" s="7" t="str">
         <f t="shared" si="21"/>
@@ -11481,7 +11338,7 @@
         <v/>
       </c>
       <c r="BV24" s="7" t="str">
-        <f t="shared" ref="AQ24:BV38" si="27">IF(BV$4=$F24,"u","")</f>
+        <f t="shared" ref="AQ24:BV32" si="27">IF(BV$4=$F24,"u","")</f>
         <v/>
       </c>
       <c r="BW24" s="7" t="str">
@@ -11494,7 +11351,7 @@
       </c>
       <c r="BY24" s="7" t="str">
         <f t="shared" si="22"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ24" s="7" t="str">
         <f t="shared" si="22"/>
@@ -11609,7 +11466,7 @@
         <v/>
       </c>
       <c r="DB24" s="7" t="str">
-        <f t="shared" ref="BW24:DB38" si="28">IF(DB$4=$F24,"u","")</f>
+        <f t="shared" ref="BW24:DB32" si="28">IF(DB$4=$F24,"u","")</f>
         <v/>
       </c>
       <c r="DC24" s="7" t="str">
@@ -11701,26 +11558,26 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:128" ht="27" customHeight="1">
+    <row r="25" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="23">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E25" s="30">
-        <v>45717</v>
+        <v>45737</v>
       </c>
       <c r="F25" s="30">
-        <v>45762</v>
+        <v>45744</v>
       </c>
       <c r="G25" s="27">
-        <f t="shared" si="25"/>
-        <v>32</v>
+        <f>IF(F25="","",NETWORKDAYS(E25,F25))</f>
+        <v>6</v>
       </c>
       <c r="H25" s="31" t="s">
         <v>12</v>
@@ -11923,7 +11780,7 @@
       </c>
       <c r="BG25" s="7" t="str">
         <f t="shared" si="27"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BH25" s="7" t="str">
         <f t="shared" si="27"/>
@@ -11995,7 +11852,7 @@
       </c>
       <c r="BY25" s="7" t="str">
         <f t="shared" si="28"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ25" s="7" t="str">
         <f t="shared" si="28"/>
@@ -12202,14 +12059,12 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:128" ht="27" customHeight="1">
+    <row r="26" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="23">
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="C26" s="24" t="s">
-        <v>25</v>
-      </c>
+      <c r="C26" s="24"/>
       <c r="D26" s="31" t="s">
         <v>19</v>
       </c>
@@ -12220,7 +12075,7 @@
         <v>45762</v>
       </c>
       <c r="G26" s="27">
-        <f t="shared" si="25"/>
+        <f>IF(F26="","",NETWORKDAYS(E26,F26))</f>
         <v>32</v>
       </c>
       <c r="H26" s="31" t="s">
@@ -12703,14 +12558,12 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:128" ht="27" customHeight="1">
+    <row r="27" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="23">
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="C27" s="24" t="s">
-        <v>26</v>
-      </c>
+      <c r="C27" s="24"/>
       <c r="D27" s="31" t="s">
         <v>16</v>
       </c>
@@ -12721,7 +12574,7 @@
         <v>45762</v>
       </c>
       <c r="G27" s="27">
-        <f t="shared" si="25"/>
+        <f>IF(F27="","",NETWORKDAYS(E27,F27))</f>
         <v>32</v>
       </c>
       <c r="H27" s="31" t="s">
@@ -13204,16 +13057,14 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:128" ht="27" customHeight="1">
+    <row r="28" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="23">
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="24"/>
+      <c r="D28" s="31" t="s">
         <v>27</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>32</v>
       </c>
       <c r="E28" s="30">
         <v>45717</v>
@@ -13222,7 +13073,7 @@
         <v>45762</v>
       </c>
       <c r="G28" s="27">
-        <f t="shared" si="25"/>
+        <f>IF(F28="","",NETWORKDAYS(E28,F28))</f>
         <v>32</v>
       </c>
       <c r="H28" s="31" t="s">
@@ -13705,16 +13556,14 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:128" ht="27" customHeight="1">
+    <row r="29" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="23">
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="C29" s="24" t="s">
-        <v>40</v>
-      </c>
+      <c r="C29" s="24"/>
       <c r="D29" s="31" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E29" s="30">
         <v>45717</v>
@@ -13723,7 +13572,7 @@
         <v>45762</v>
       </c>
       <c r="G29" s="27">
-        <f t="shared" si="25"/>
+        <f>IF(F29="","",NETWORKDAYS(E29,F29))</f>
         <v>32</v>
       </c>
       <c r="H29" s="31" t="s">
@@ -14206,7 +14055,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:128" ht="27" customHeight="1">
+    <row r="30" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="23">
         <f t="shared" si="6"/>
         <v>25</v>
@@ -14692,7 +14541,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:128" ht="27" customHeight="1">
+    <row r="31" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="23">
         <f t="shared" si="6"/>
         <v>26</v>
@@ -15178,7 +15027,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:128" ht="27" customHeight="1">
+    <row r="32" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="23">
         <f t="shared" si="6"/>
         <v>27</v>
@@ -15312,7 +15161,7 @@
         <v/>
       </c>
       <c r="AO32" s="7" t="str">
-        <f t="shared" ref="AO32:AP38" si="31">IF(AO$4=$F32,"u","")</f>
+        <f t="shared" ref="AO32:AP32" si="31">IF(AO$4=$F32,"u","")</f>
         <v/>
       </c>
       <c r="AP32" s="7" t="str">
@@ -15440,7 +15289,7 @@
         <v/>
       </c>
       <c r="BU32" s="7" t="str">
-        <f t="shared" ref="BU32:BV38" si="32">IF(BU$4=$F32,"u","")</f>
+        <f t="shared" ref="BU32:BV32" si="32">IF(BU$4=$F32,"u","")</f>
         <v/>
       </c>
       <c r="BV32" s="7" t="str">
@@ -15568,7 +15417,7 @@
         <v/>
       </c>
       <c r="DA32" s="7" t="str">
-        <f t="shared" ref="DA32:DB38" si="33">IF(DA$4=$F32,"u","")</f>
+        <f t="shared" ref="DA32:DB32" si="33">IF(DA$4=$F32,"u","")</f>
         <v/>
       </c>
       <c r="DB32" s="7" t="str">
@@ -15664,7 +15513,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:128" ht="27" customHeight="1">
+    <row r="33" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="23">
         <f t="shared" si="6"/>
         <v>28</v>
@@ -16150,7 +15999,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:128" ht="27" customHeight="1">
+    <row r="34" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B34" s="23">
         <f t="shared" si="6"/>
         <v>29</v>
@@ -16636,7 +16485,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:128" ht="27" customHeight="1">
+    <row r="35" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B35" s="23">
         <f t="shared" si="6"/>
         <v>30</v>
@@ -17122,7 +16971,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:128" ht="27" customHeight="1">
+    <row r="36" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" s="23">
         <f t="shared" si="6"/>
         <v>31</v>
@@ -17608,7 +17457,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:128" ht="27" customHeight="1">
+    <row r="37" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="23">
         <f t="shared" si="6"/>
         <v>32</v>
@@ -18094,7 +17943,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:128" ht="27" customHeight="1">
+    <row r="38" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B38" s="23">
         <f t="shared" si="6"/>
         <v>33</v>
@@ -18580,28 +18429,28 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:128" ht="17" thickBot="1"/>
-    <row r="43" spans="2:128" ht="17" thickBot="1">
+    <row r="42" spans="2:128" ht="16.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="2:128" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C43" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="2:128">
+    <row r="44" spans="2:128" x14ac:dyDescent="0.4">
       <c r="C44" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="2:128">
+    <row r="45" spans="2:128" x14ac:dyDescent="0.4">
       <c r="C45" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="2:128">
+    <row r="46" spans="2:128" x14ac:dyDescent="0.4">
       <c r="C46" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="2:128" ht="17" thickBot="1">
+    <row r="47" spans="2:128" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C47" s="13" t="s">
         <v>15</v>
       </c>
@@ -18619,7 +18468,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H6:H38">
-    <cfRule type="containsText" dxfId="31" priority="8" operator="containsText" text="Blocked">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Blocked">
       <formula>NOT(ISERROR(SEARCH("Blocked",H6)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18638,49 +18487,47 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:DX38">
-    <cfRule type="expression" dxfId="30" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>AND($H6="Blocked",$I6&gt;0,K$4&lt;=($E6+($F6-$E6)*($I6)),K$4&gt;=$E6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>AND($H6="Complete",K$4=$F6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>AND($I6&gt;0,K$4&lt;=($E6+($F6-$E6)*$I6),K$4&gt;=$E6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>AND(K$4&gt;=$E6,K$4&lt;=$F6)</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K6:DX38">
-    <cfRule type="expression" dxfId="26" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>K$4=(TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28:CN38">
-    <cfRule type="expression" dxfId="25" priority="46">
+    <cfRule type="expression" dxfId="7" priority="46">
       <formula>AND($H31="Blocked",$I31&gt;0,L$4&lt;=($E31+($F31-$E31)*($I31)),L$4&gt;=$E31)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="47">
+    <cfRule type="expression" dxfId="6" priority="47">
       <formula>AND($H31="Complete",L$4=$F31)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="48">
+    <cfRule type="expression" dxfId="5" priority="48">
       <formula>AND($I31&gt;0,L$4&lt;=($E31+($F31-$E31)*$I31),L$4&gt;=$E31)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="49">
+    <cfRule type="expression" dxfId="4" priority="49">
       <formula>AND(L$4&gt;=$E31,L$4&lt;=$F31)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CO25:DX38">
-    <cfRule type="expression" dxfId="21" priority="61">
+    <cfRule type="expression" dxfId="3" priority="61">
       <formula>AND($H24="Blocked",$I24&gt;0,CO$4&lt;=($E24+($F24-$E24)*($I24)),CO$4&gt;=$E24)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="62">
+    <cfRule type="expression" dxfId="2" priority="62">
       <formula>AND($H24="Complete",CO$4=$F24)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="63">
+    <cfRule type="expression" dxfId="1" priority="63">
       <formula>AND($I24&gt;0,CO$4&lt;=($E24+($F24-$E24)*$I24),CO$4&gt;=$E24)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="64">
+    <cfRule type="expression" dxfId="0" priority="64">
       <formula>AND(CO$4&gt;=$E24,CO$4&lt;=$F24)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixed animation error when enemies walking down direction and updated the gant chart
</commit_message>
<xml_diff>
--- a/docs/GantChart_Azelele_MGuz.xlsx
+++ b/docs/GantChart_Azelele_MGuz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muratguzelocak/Documents/Projects/FreeBomber/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184DE38E-C86E-FA43-A3B1-52AA9E2FB30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4207A571-0C82-0E4F-BD29-A2E5DA7552DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>Project Start Date:</t>
   </si>
@@ -151,6 +151,9 @@
   <si>
     <t>Comment Character and JackBomber Classes</t>
   </si>
+  <si>
+    <t xml:space="preserve"> i</t>
+  </si>
 </sst>
 </file>
 
@@ -237,7 +240,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +280,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9EF8FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,7 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
@@ -647,6 +656,9 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1095,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF3DB2-1A6B-144B-8344-5E254C7EE240}">
   <dimension ref="A1:DX47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16"/>
@@ -1711,7 +1723,7 @@
         <f t="shared" si="1"/>
         <v>45767</v>
       </c>
-      <c r="CE4" s="6">
+      <c r="CE4" s="43">
         <f t="shared" si="1"/>
         <v>45768</v>
       </c>
@@ -5914,9 +5926,8 @@
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="CR13" s="7" t="str">
-        <f t="shared" si="15"/>
-        <v/>
+      <c r="CR13" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="CS13" s="7" t="str">
         <f t="shared" si="15"/>
@@ -8073,10 +8084,10 @@
         <v>11</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I18" s="32">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="7" t="str">
@@ -9065,10 +9076,10 @@
         <v>16</v>
       </c>
       <c r="E20" s="30">
+        <v>45737</v>
+      </c>
+      <c r="F20" s="30">
         <v>45744</v>
-      </c>
-      <c r="F20" s="30">
-        <v>45751</v>
       </c>
       <c r="G20" s="27">
         <f t="shared" si="25"/>
@@ -9275,7 +9286,7 @@
       </c>
       <c r="BG20" s="7" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BH20" s="7" t="str">
         <f t="shared" si="21"/>
@@ -9303,7 +9314,7 @@
       </c>
       <c r="BN20" s="7" t="str">
         <f t="shared" si="21"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BO20" s="7" t="str">
         <f t="shared" si="21"/>
@@ -12082,7 +12093,7 @@
         <v>12</v>
       </c>
       <c r="I26" s="32">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="7" t="str">

</xml_diff>

<commit_message>
added the special door
</commit_message>
<xml_diff>
--- a/docs/GantChart_Azelele_MGuz.xlsx
+++ b/docs/GantChart_Azelele_MGuz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muratguzelocak/Documents/Projects/FreeBomber/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\FinalProject\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4207A571-0C82-0E4F-BD29-A2E5DA7552DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE28266F-D519-4D75-A2B6-61FBDA5D9A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>Project Start Date:</t>
   </si>
@@ -154,6 +154,12 @@
   <si>
     <t xml:space="preserve"> i</t>
   </si>
+  <si>
+    <t>limit the Players health and display it on the screen with level number and timer</t>
+  </si>
+  <si>
+    <t>Create the game intro and score keeping</t>
+  </si>
 </sst>
 </file>
 
@@ -165,7 +171,7 @@
     <numFmt numFmtId="166" formatCode="mmm\-d\-yy"/>
     <numFmt numFmtId="167" formatCode="mmm\-d"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -547,7 +553,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
@@ -633,6 +639,9 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -657,9 +666,7 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1107,11 +1114,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF3DB2-1A6B-144B-8344-5E254C7EE240}">
   <dimension ref="A1:DX47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:I29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScale="48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
@@ -1136,8 +1143,8 @@
     <col min="77" max="77" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:128" ht="54" customHeight="1" thickBot="1"/>
-    <row r="2" spans="1:128" ht="25" thickBot="1">
+    <row r="1" spans="1:128" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:128" ht="24" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -1147,132 +1154,132 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
-      <c r="K2" s="37">
+      <c r="K2" s="38">
         <f>K3</f>
         <v>45697</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="37"/>
-      <c r="AK2" s="37"/>
-      <c r="AL2" s="37"/>
-      <c r="AM2" s="37"/>
-      <c r="AN2" s="37"/>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
-      <c r="AQ2" s="37"/>
-      <c r="AR2" s="37"/>
-      <c r="AS2" s="37"/>
-      <c r="AT2" s="37"/>
-      <c r="AU2" s="37"/>
-      <c r="AV2" s="37"/>
-      <c r="AW2" s="37"/>
-      <c r="AX2" s="37"/>
-      <c r="AY2" s="37"/>
-      <c r="AZ2" s="37"/>
-      <c r="BA2" s="37"/>
-      <c r="BB2" s="37"/>
-      <c r="BC2" s="37"/>
-      <c r="BD2" s="37"/>
-      <c r="BE2" s="37"/>
-      <c r="BF2" s="37"/>
-      <c r="BG2" s="37"/>
-      <c r="BH2" s="37"/>
-      <c r="BI2" s="37"/>
-      <c r="BJ2" s="37"/>
-      <c r="BK2" s="37"/>
-      <c r="BL2" s="37"/>
-      <c r="BM2" s="37"/>
-      <c r="BN2" s="37"/>
-      <c r="BO2" s="37"/>
-      <c r="BP2" s="37"/>
-      <c r="BQ2" s="38">
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
+      <c r="AQ2" s="38"/>
+      <c r="AR2" s="38"/>
+      <c r="AS2" s="38"/>
+      <c r="AT2" s="38"/>
+      <c r="AU2" s="38"/>
+      <c r="AV2" s="38"/>
+      <c r="AW2" s="38"/>
+      <c r="AX2" s="38"/>
+      <c r="AY2" s="38"/>
+      <c r="AZ2" s="38"/>
+      <c r="BA2" s="38"/>
+      <c r="BB2" s="38"/>
+      <c r="BC2" s="38"/>
+      <c r="BD2" s="38"/>
+      <c r="BE2" s="38"/>
+      <c r="BF2" s="38"/>
+      <c r="BG2" s="38"/>
+      <c r="BH2" s="38"/>
+      <c r="BI2" s="38"/>
+      <c r="BJ2" s="38"/>
+      <c r="BK2" s="38"/>
+      <c r="BL2" s="38"/>
+      <c r="BM2" s="38"/>
+      <c r="BN2" s="38"/>
+      <c r="BO2" s="38"/>
+      <c r="BP2" s="38"/>
+      <c r="BQ2" s="39">
         <f>BQ3</f>
         <v>45769</v>
       </c>
-      <c r="BR2" s="38"/>
-      <c r="BS2" s="38"/>
-      <c r="BT2" s="38"/>
-      <c r="BU2" s="38"/>
-      <c r="BV2" s="38"/>
-      <c r="BW2" s="38"/>
-      <c r="BX2" s="38"/>
-      <c r="BY2" s="38"/>
-      <c r="BZ2" s="38"/>
-      <c r="CA2" s="38"/>
-      <c r="CB2" s="38"/>
-      <c r="CC2" s="38"/>
-      <c r="CD2" s="38"/>
-      <c r="CE2" s="38"/>
-      <c r="CF2" s="38"/>
-      <c r="CG2" s="38"/>
-      <c r="CH2" s="38"/>
-      <c r="CI2" s="38"/>
-      <c r="CJ2" s="38"/>
-      <c r="CK2" s="38"/>
-      <c r="CL2" s="38"/>
-      <c r="CM2" s="38"/>
-      <c r="CN2" s="38"/>
-      <c r="CO2" s="38"/>
-      <c r="CP2" s="38"/>
-      <c r="CQ2" s="38"/>
-      <c r="CR2" s="38"/>
-      <c r="CS2" s="38"/>
-      <c r="CT2" s="38"/>
-      <c r="CU2" s="38"/>
-      <c r="CV2" s="38"/>
-      <c r="CW2" s="38"/>
-      <c r="CX2" s="38"/>
-      <c r="CY2" s="38"/>
-      <c r="CZ2" s="38"/>
-      <c r="DA2" s="38"/>
-      <c r="DB2" s="38"/>
-      <c r="DC2" s="38"/>
-      <c r="DD2" s="38"/>
-      <c r="DE2" s="38"/>
-      <c r="DF2" s="38"/>
-      <c r="DG2" s="38"/>
-      <c r="DH2" s="38"/>
-      <c r="DI2" s="38"/>
-      <c r="DJ2" s="38"/>
-      <c r="DK2" s="38"/>
-      <c r="DL2" s="38"/>
-      <c r="DM2" s="38"/>
-      <c r="DN2" s="38"/>
-      <c r="DO2" s="38"/>
-      <c r="DP2" s="38"/>
-      <c r="DQ2" s="38"/>
-      <c r="DR2" s="38"/>
-      <c r="DS2" s="38"/>
-      <c r="DT2" s="38"/>
-      <c r="DU2" s="38"/>
-      <c r="DV2" s="38"/>
-      <c r="DW2" s="38"/>
-      <c r="DX2" s="39"/>
+      <c r="BR2" s="39"/>
+      <c r="BS2" s="39"/>
+      <c r="BT2" s="39"/>
+      <c r="BU2" s="39"/>
+      <c r="BV2" s="39"/>
+      <c r="BW2" s="39"/>
+      <c r="BX2" s="39"/>
+      <c r="BY2" s="39"/>
+      <c r="BZ2" s="39"/>
+      <c r="CA2" s="39"/>
+      <c r="CB2" s="39"/>
+      <c r="CC2" s="39"/>
+      <c r="CD2" s="39"/>
+      <c r="CE2" s="39"/>
+      <c r="CF2" s="39"/>
+      <c r="CG2" s="39"/>
+      <c r="CH2" s="39"/>
+      <c r="CI2" s="39"/>
+      <c r="CJ2" s="39"/>
+      <c r="CK2" s="39"/>
+      <c r="CL2" s="39"/>
+      <c r="CM2" s="39"/>
+      <c r="CN2" s="39"/>
+      <c r="CO2" s="39"/>
+      <c r="CP2" s="39"/>
+      <c r="CQ2" s="39"/>
+      <c r="CR2" s="39"/>
+      <c r="CS2" s="39"/>
+      <c r="CT2" s="39"/>
+      <c r="CU2" s="39"/>
+      <c r="CV2" s="39"/>
+      <c r="CW2" s="39"/>
+      <c r="CX2" s="39"/>
+      <c r="CY2" s="39"/>
+      <c r="CZ2" s="39"/>
+      <c r="DA2" s="39"/>
+      <c r="DB2" s="39"/>
+      <c r="DC2" s="39"/>
+      <c r="DD2" s="39"/>
+      <c r="DE2" s="39"/>
+      <c r="DF2" s="39"/>
+      <c r="DG2" s="39"/>
+      <c r="DH2" s="39"/>
+      <c r="DI2" s="39"/>
+      <c r="DJ2" s="39"/>
+      <c r="DK2" s="39"/>
+      <c r="DL2" s="39"/>
+      <c r="DM2" s="39"/>
+      <c r="DN2" s="39"/>
+      <c r="DO2" s="39"/>
+      <c r="DP2" s="39"/>
+      <c r="DQ2" s="39"/>
+      <c r="DR2" s="39"/>
+      <c r="DS2" s="39"/>
+      <c r="DT2" s="39"/>
+      <c r="DU2" s="39"/>
+      <c r="DV2" s="39"/>
+      <c r="DW2" s="39"/>
+      <c r="DX2" s="40"/>
     </row>
-    <row r="3" spans="1:128" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
+    <row r="3" spans="1:128" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3"/>
       <c r="B3" s="15"/>
       <c r="C3" s="33" t="s">
@@ -1287,153 +1294,153 @@
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3"/>
-      <c r="K3" s="42">
+      <c r="K3" s="43">
         <f>L4</f>
         <v>45697</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="42"/>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="42"/>
-      <c r="X3" s="42"/>
-      <c r="Y3" s="42"/>
-      <c r="Z3" s="42"/>
-      <c r="AA3" s="42"/>
-      <c r="AB3" s="42"/>
-      <c r="AC3" s="42"/>
-      <c r="AD3" s="42"/>
-      <c r="AE3" s="42"/>
-      <c r="AF3" s="42"/>
-      <c r="AG3" s="42"/>
-      <c r="AH3" s="42"/>
-      <c r="AI3" s="42"/>
-      <c r="AJ3" s="42"/>
-      <c r="AK3" s="42"/>
-      <c r="AL3" s="35">
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="43"/>
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="43"/>
+      <c r="AD3" s="43"/>
+      <c r="AE3" s="43"/>
+      <c r="AF3" s="43"/>
+      <c r="AG3" s="43"/>
+      <c r="AH3" s="43"/>
+      <c r="AI3" s="43"/>
+      <c r="AJ3" s="43"/>
+      <c r="AK3" s="43"/>
+      <c r="AL3" s="36">
         <f>AZ4</f>
         <v>45737</v>
       </c>
-      <c r="AM3" s="35"/>
-      <c r="AN3" s="35"/>
-      <c r="AO3" s="35"/>
-      <c r="AP3" s="35"/>
-      <c r="AQ3" s="35"/>
-      <c r="AR3" s="35"/>
-      <c r="AS3" s="35"/>
-      <c r="AT3" s="35"/>
-      <c r="AU3" s="35"/>
-      <c r="AV3" s="35"/>
-      <c r="AW3" s="35"/>
-      <c r="AX3" s="35"/>
-      <c r="AY3" s="35"/>
-      <c r="AZ3" s="35"/>
-      <c r="BA3" s="35"/>
-      <c r="BB3" s="35"/>
-      <c r="BC3" s="35"/>
-      <c r="BD3" s="35"/>
-      <c r="BE3" s="35"/>
-      <c r="BF3" s="35"/>
-      <c r="BG3" s="35"/>
-      <c r="BH3" s="35"/>
-      <c r="BI3" s="35"/>
-      <c r="BJ3" s="35"/>
-      <c r="BK3" s="35"/>
-      <c r="BL3" s="35"/>
-      <c r="BM3" s="35"/>
-      <c r="BN3" s="35"/>
-      <c r="BO3" s="35"/>
-      <c r="BP3" s="35"/>
-      <c r="BQ3" s="42">
+      <c r="AM3" s="36"/>
+      <c r="AN3" s="36"/>
+      <c r="AO3" s="36"/>
+      <c r="AP3" s="36"/>
+      <c r="AQ3" s="36"/>
+      <c r="AR3" s="36"/>
+      <c r="AS3" s="36"/>
+      <c r="AT3" s="36"/>
+      <c r="AU3" s="36"/>
+      <c r="AV3" s="36"/>
+      <c r="AW3" s="36"/>
+      <c r="AX3" s="36"/>
+      <c r="AY3" s="36"/>
+      <c r="AZ3" s="36"/>
+      <c r="BA3" s="36"/>
+      <c r="BB3" s="36"/>
+      <c r="BC3" s="36"/>
+      <c r="BD3" s="36"/>
+      <c r="BE3" s="36"/>
+      <c r="BF3" s="36"/>
+      <c r="BG3" s="36"/>
+      <c r="BH3" s="36"/>
+      <c r="BI3" s="36"/>
+      <c r="BJ3" s="36"/>
+      <c r="BK3" s="36"/>
+      <c r="BL3" s="36"/>
+      <c r="BM3" s="36"/>
+      <c r="BN3" s="36"/>
+      <c r="BO3" s="36"/>
+      <c r="BP3" s="36"/>
+      <c r="BQ3" s="43">
         <f>CF4</f>
         <v>45769</v>
       </c>
-      <c r="BR3" s="42"/>
-      <c r="BS3" s="42"/>
-      <c r="BT3" s="42"/>
-      <c r="BU3" s="42"/>
-      <c r="BV3" s="42"/>
-      <c r="BW3" s="42"/>
-      <c r="BX3" s="42"/>
-      <c r="BY3" s="42"/>
-      <c r="BZ3" s="42"/>
-      <c r="CA3" s="42"/>
-      <c r="CB3" s="42"/>
-      <c r="CC3" s="42"/>
-      <c r="CD3" s="42"/>
-      <c r="CE3" s="42"/>
-      <c r="CF3" s="42"/>
-      <c r="CG3" s="42"/>
-      <c r="CH3" s="42"/>
-      <c r="CI3" s="42"/>
-      <c r="CJ3" s="42"/>
-      <c r="CK3" s="42"/>
-      <c r="CL3" s="42"/>
-      <c r="CM3" s="42"/>
-      <c r="CN3" s="42"/>
-      <c r="CO3" s="42"/>
-      <c r="CP3" s="42"/>
-      <c r="CQ3" s="42"/>
-      <c r="CR3" s="42"/>
-      <c r="CS3" s="42"/>
-      <c r="CT3" s="42"/>
-      <c r="CU3" s="35">
+      <c r="BR3" s="43"/>
+      <c r="BS3" s="43"/>
+      <c r="BT3" s="43"/>
+      <c r="BU3" s="43"/>
+      <c r="BV3" s="43"/>
+      <c r="BW3" s="43"/>
+      <c r="BX3" s="43"/>
+      <c r="BY3" s="43"/>
+      <c r="BZ3" s="43"/>
+      <c r="CA3" s="43"/>
+      <c r="CB3" s="43"/>
+      <c r="CC3" s="43"/>
+      <c r="CD3" s="43"/>
+      <c r="CE3" s="43"/>
+      <c r="CF3" s="43"/>
+      <c r="CG3" s="43"/>
+      <c r="CH3" s="43"/>
+      <c r="CI3" s="43"/>
+      <c r="CJ3" s="43"/>
+      <c r="CK3" s="43"/>
+      <c r="CL3" s="43"/>
+      <c r="CM3" s="43"/>
+      <c r="CN3" s="43"/>
+      <c r="CO3" s="43"/>
+      <c r="CP3" s="43"/>
+      <c r="CQ3" s="43"/>
+      <c r="CR3" s="43"/>
+      <c r="CS3" s="43"/>
+      <c r="CT3" s="43"/>
+      <c r="CU3" s="36">
         <f>DJ4</f>
         <v>45799</v>
       </c>
-      <c r="CV3" s="35"/>
-      <c r="CW3" s="35"/>
-      <c r="CX3" s="35"/>
-      <c r="CY3" s="35"/>
-      <c r="CZ3" s="35"/>
-      <c r="DA3" s="35"/>
-      <c r="DB3" s="35"/>
-      <c r="DC3" s="35"/>
-      <c r="DD3" s="35"/>
-      <c r="DE3" s="35"/>
-      <c r="DF3" s="35"/>
-      <c r="DG3" s="35"/>
-      <c r="DH3" s="35"/>
-      <c r="DI3" s="35"/>
-      <c r="DJ3" s="35"/>
-      <c r="DK3" s="35"/>
-      <c r="DL3" s="35"/>
-      <c r="DM3" s="35"/>
-      <c r="DN3" s="35"/>
-      <c r="DO3" s="35"/>
-      <c r="DP3" s="35"/>
-      <c r="DQ3" s="35"/>
-      <c r="DR3" s="35"/>
-      <c r="DS3" s="35"/>
-      <c r="DT3" s="35"/>
-      <c r="DU3" s="35"/>
-      <c r="DV3" s="35"/>
-      <c r="DW3" s="35"/>
-      <c r="DX3" s="36"/>
+      <c r="CV3" s="36"/>
+      <c r="CW3" s="36"/>
+      <c r="CX3" s="36"/>
+      <c r="CY3" s="36"/>
+      <c r="CZ3" s="36"/>
+      <c r="DA3" s="36"/>
+      <c r="DB3" s="36"/>
+      <c r="DC3" s="36"/>
+      <c r="DD3" s="36"/>
+      <c r="DE3" s="36"/>
+      <c r="DF3" s="36"/>
+      <c r="DG3" s="36"/>
+      <c r="DH3" s="36"/>
+      <c r="DI3" s="36"/>
+      <c r="DJ3" s="36"/>
+      <c r="DK3" s="36"/>
+      <c r="DL3" s="36"/>
+      <c r="DM3" s="36"/>
+      <c r="DN3" s="36"/>
+      <c r="DO3" s="36"/>
+      <c r="DP3" s="36"/>
+      <c r="DQ3" s="36"/>
+      <c r="DR3" s="36"/>
+      <c r="DS3" s="36"/>
+      <c r="DT3" s="36"/>
+      <c r="DU3" s="36"/>
+      <c r="DV3" s="36"/>
+      <c r="DW3" s="36"/>
+      <c r="DX3" s="37"/>
     </row>
-    <row r="4" spans="1:128" s="1" customFormat="1" ht="41" customHeight="1">
+    <row r="4" spans="1:128" s="1" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4"/>
       <c r="B4" s="18"/>
       <c r="C4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="40" t="s">
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="40"/>
+      <c r="I4" s="41"/>
       <c r="J4"/>
       <c r="K4" s="5">
         <f>D3</f>
@@ -1723,7 +1730,7 @@
         <f t="shared" si="1"/>
         <v>45767</v>
       </c>
-      <c r="CE4" s="43">
+      <c r="CE4" s="35">
         <f t="shared" si="1"/>
         <v>45768</v>
       </c>
@@ -1908,7 +1915,7 @@
         <v>45813</v>
       </c>
     </row>
-    <row r="5" spans="1:128" ht="23">
+    <row r="5" spans="1:128" ht="25.5" x14ac:dyDescent="0.4">
       <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
@@ -2053,7 +2060,7 @@
       <c r="DW5" s="4"/>
       <c r="DX5" s="11"/>
     </row>
-    <row r="6" spans="1:128" ht="27" customHeight="1">
+    <row r="6" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="23">
         <v>1</v>
       </c>
@@ -2552,7 +2559,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:128" ht="27" customHeight="1">
+    <row r="7" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="23">
         <f>B6+1</f>
         <v>2</v>
@@ -3053,7 +3060,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:128" ht="27" customHeight="1">
+    <row r="8" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="23">
         <f t="shared" ref="B8:B38" si="6">B7+1</f>
         <v>3</v>
@@ -3554,7 +3561,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:128" ht="27" customHeight="1">
+    <row r="9" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="23">
         <f t="shared" si="6"/>
         <v>4</v>
@@ -4055,7 +4062,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:128" ht="27" customHeight="1">
+    <row r="10" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="23">
         <f t="shared" si="6"/>
         <v>5</v>
@@ -4070,11 +4077,11 @@
         <v>45716</v>
       </c>
       <c r="F10" s="30">
-        <v>45737</v>
+        <v>45745</v>
       </c>
       <c r="G10" s="27">
         <f t="shared" ref="G10" si="8">IF(F10="","",NETWORKDAYS(E10,F10))</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H10" s="31" t="s">
         <v>13</v>
@@ -4249,39 +4256,39 @@
       </c>
       <c r="AZ10" s="7" t="str">
         <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="BA10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="BB10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="BC10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="BD10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="BE10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="BF10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="BG10" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="BH10" s="7" t="str">
+        <f t="shared" si="7"/>
         <v>u</v>
-      </c>
-      <c r="BA10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="BB10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="BC10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="BD10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="BE10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="BF10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="BG10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="BH10" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v/>
       </c>
       <c r="BI10" s="7" t="str">
         <f t="shared" si="7"/>
@@ -4556,7 +4563,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:128" ht="27" customHeight="1">
+    <row r="11" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="23">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -5057,7 +5064,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:128" ht="27" customHeight="1">
+    <row r="12" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="23">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -5558,7 +5565,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:128" ht="27" customHeight="1">
+    <row r="13" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="23">
         <f t="shared" si="6"/>
         <v>8</v>
@@ -6058,7 +6065,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:128" ht="27" customHeight="1">
+    <row r="14" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="23">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -6559,7 +6566,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:128" ht="27" customHeight="1">
+    <row r="15" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="23">
         <f t="shared" si="6"/>
         <v>10</v>
@@ -7060,7 +7067,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:128" ht="27" customHeight="1">
+    <row r="16" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="23">
         <f t="shared" si="6"/>
         <v>11</v>
@@ -7075,17 +7082,17 @@
         <v>45734</v>
       </c>
       <c r="F16" s="30">
-        <v>45741</v>
+        <v>45757</v>
       </c>
       <c r="G16" s="27">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="H16" s="31" t="s">
         <v>13</v>
       </c>
       <c r="I16" s="32">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="7" t="str">
@@ -7270,7 +7277,7 @@
       </c>
       <c r="BD16" s="7" t="str">
         <f t="shared" si="17"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BE16" s="7" t="str">
         <f t="shared" si="17"/>
@@ -7334,7 +7341,7 @@
       </c>
       <c r="BT16" s="7" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BU16" s="7" t="str">
         <f t="shared" si="18"/>
@@ -7561,7 +7568,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:128" ht="27" customHeight="1">
+    <row r="17" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="23">
         <f t="shared" si="6"/>
         <v>12</v>
@@ -7583,10 +7590,10 @@
         <v>6</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I17" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="7" t="str">
@@ -8062,7 +8069,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:128" ht="27" customHeight="1">
+    <row r="18" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="23">
         <f t="shared" si="6"/>
         <v>13</v>
@@ -8563,7 +8570,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:128" ht="27" customHeight="1">
+    <row r="19" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="23">
         <f t="shared" si="6"/>
         <v>14</v>
@@ -9064,7 +9071,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:128" ht="27" customHeight="1">
+    <row r="20" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="23">
         <f t="shared" si="6"/>
         <v>15</v>
@@ -9086,10 +9093,10 @@
         <v>6</v>
       </c>
       <c r="H20" s="31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I20" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="7" t="str">
@@ -9565,7 +9572,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:128" ht="27" customHeight="1">
+    <row r="21" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="23">
         <f t="shared" si="6"/>
         <v>16</v>
@@ -9577,17 +9584,17 @@
         <v>27</v>
       </c>
       <c r="E21" s="30">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="F21" s="30">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="G21" s="27">
         <f t="shared" ref="G21:G29" si="26">IF(F21="","",NETWORKDAYS(E21,F21))</f>
         <v>1</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I21" s="32">
         <v>0.5</v>
@@ -9771,20 +9778,20 @@
       </c>
       <c r="BC21" s="7" t="str">
         <f>IF(BC$4=$F21,"u","")</f>
+        <v/>
+      </c>
+      <c r="BD21" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BE21" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BF21" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>u</v>
       </c>
-      <c r="BD21" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BE21" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BF21" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
       <c r="BG21" s="7" t="str">
         <f t="shared" si="21"/>
         <v/>
@@ -10066,7 +10073,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:128" ht="27" customHeight="1">
+    <row r="22" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="23">
         <f t="shared" si="6"/>
         <v>17</v>
@@ -10088,10 +10095,10 @@
         <v>5</v>
       </c>
       <c r="H22" s="31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I22" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="7" t="str">
@@ -10567,7 +10574,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:128" ht="27" customHeight="1">
+    <row r="23" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="23">
         <f t="shared" si="6"/>
         <v>18</v>
@@ -10579,14 +10586,14 @@
         <v>16</v>
       </c>
       <c r="E23" s="30">
-        <v>45737</v>
+        <v>45743</v>
       </c>
       <c r="F23" s="30">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="G23" s="27">
         <f t="shared" si="26"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H23" s="31" t="s">
         <v>12</v>
@@ -10789,20 +10796,20 @@
       </c>
       <c r="BG23" s="7" t="str">
         <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BH23" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BI23" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BJ23" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>u</v>
       </c>
-      <c r="BH23" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BI23" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BJ23" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
       <c r="BK23" s="7" t="str">
         <f t="shared" si="21"/>
         <v/>
@@ -11068,7 +11075,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:128" ht="27" customHeight="1">
+    <row r="24" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="23">
         <f t="shared" si="6"/>
         <v>19</v>
@@ -11093,7 +11100,7 @@
         <v>12</v>
       </c>
       <c r="I24" s="32">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="7" t="str">
@@ -11105,7 +11112,7 @@
         <v/>
       </c>
       <c r="M24" s="7" t="str">
-        <f t="shared" si="20"/>
+        <f>IF(M$4=$F24,"u","")</f>
         <v/>
       </c>
       <c r="N24" s="7" t="str">
@@ -11569,7 +11576,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:128" ht="27" customHeight="1">
+    <row r="25" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="23">
         <f t="shared" si="6"/>
         <v>20</v>
@@ -12070,24 +12077,26 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:128" ht="27" customHeight="1">
+    <row r="26" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="23">
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="C26" s="24"/>
+      <c r="C26" s="24" t="s">
+        <v>39</v>
+      </c>
       <c r="D26" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="30">
-        <v>45717</v>
+        <v>45745</v>
       </c>
       <c r="F26" s="30">
-        <v>45762</v>
+        <v>45751</v>
       </c>
       <c r="G26" s="27">
         <f t="shared" si="26"/>
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="H26" s="31" t="s">
         <v>12</v>
@@ -12318,7 +12327,7 @@
       </c>
       <c r="BN26" s="7" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BO26" s="7" t="str">
         <f t="shared" si="28"/>
@@ -12362,7 +12371,7 @@
       </c>
       <c r="BY26" s="7" t="str">
         <f t="shared" si="29"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ26" s="7" t="str">
         <f t="shared" si="29"/>
@@ -12569,24 +12578,26 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:128" ht="27" customHeight="1">
+    <row r="27" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B27" s="23">
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="C27" s="24"/>
+      <c r="C27" s="44" t="s">
+        <v>40</v>
+      </c>
       <c r="D27" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="30">
-        <v>45717</v>
+        <v>45745</v>
       </c>
       <c r="F27" s="30">
-        <v>45762</v>
+        <v>45751</v>
       </c>
       <c r="G27" s="27">
         <f t="shared" si="26"/>
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="H27" s="31" t="s">
         <v>12</v>
@@ -12817,7 +12828,7 @@
       </c>
       <c r="BN27" s="7" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BO27" s="7" t="str">
         <f t="shared" si="28"/>
@@ -12861,7 +12872,7 @@
       </c>
       <c r="BY27" s="7" t="str">
         <f t="shared" si="29"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ27" s="7" t="str">
         <f t="shared" si="29"/>
@@ -13068,7 +13079,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:128" ht="27" customHeight="1">
+    <row r="28" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="23">
         <f t="shared" si="6"/>
         <v>23</v>
@@ -13567,7 +13578,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:128" ht="27" customHeight="1">
+    <row r="29" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="23">
         <f t="shared" si="6"/>
         <v>24</v>
@@ -14066,7 +14077,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:128" ht="27" customHeight="1">
+    <row r="30" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="23">
         <f t="shared" si="6"/>
         <v>25</v>
@@ -14552,7 +14563,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:128" ht="27" customHeight="1">
+    <row r="31" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="23">
         <f t="shared" si="6"/>
         <v>26</v>
@@ -15038,7 +15049,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:128" ht="27" customHeight="1">
+    <row r="32" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="23">
         <f t="shared" si="6"/>
         <v>27</v>
@@ -15524,7 +15535,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:128" ht="27" customHeight="1">
+    <row r="33" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="23">
         <f t="shared" si="6"/>
         <v>28</v>
@@ -16010,7 +16021,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:128" ht="27" customHeight="1">
+    <row r="34" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B34" s="23">
         <f t="shared" si="6"/>
         <v>29</v>
@@ -16496,7 +16507,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:128" ht="27" customHeight="1">
+    <row r="35" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B35" s="23">
         <f t="shared" si="6"/>
         <v>30</v>
@@ -16982,7 +16993,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:128" ht="27" customHeight="1">
+    <row r="36" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" s="23">
         <f t="shared" si="6"/>
         <v>31</v>
@@ -17468,7 +17479,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:128" ht="27" customHeight="1">
+    <row r="37" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="23">
         <f t="shared" si="6"/>
         <v>32</v>
@@ -17954,7 +17965,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:128" ht="27" customHeight="1">
+    <row r="38" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B38" s="23">
         <f t="shared" si="6"/>
         <v>33</v>
@@ -18440,28 +18451,28 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:128" ht="17" thickBot="1"/>
-    <row r="43" spans="2:128" ht="17" thickBot="1">
+    <row r="42" spans="2:128" ht="16.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="2:128" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C43" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="2:128">
+    <row r="44" spans="2:128" x14ac:dyDescent="0.4">
       <c r="C44" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="2:128">
+    <row r="45" spans="2:128" x14ac:dyDescent="0.4">
       <c r="C45" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="2:128">
+    <row r="46" spans="2:128" x14ac:dyDescent="0.4">
       <c r="C46" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="2:128" ht="17" thickBot="1">
+    <row r="47" spans="2:128" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C47" s="13" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Updated the Gant Chart
</commit_message>
<xml_diff>
--- a/docs/GantChart_Azelele_MGuz.xlsx
+++ b/docs/GantChart_Azelele_MGuz.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muratguzelocak/Documents/Projects/FreeBomber/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4207A571-0C82-0E4F-BD29-A2E5DA7552DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B113452A-B5B2-9844-8A9D-52D42346618B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
   <si>
     <t>Project Start Date:</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Vision Statement Write-Up</t>
   </si>
   <si>
-    <t>Champ. Player Special Abilities Dev</t>
-  </si>
-  <si>
     <t>Both</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>Comment Background and Tile Manager Class</t>
   </si>
   <si>
-    <t>Special door Dev</t>
-  </si>
-  <si>
     <t>Comment all Enemy Classes</t>
   </si>
   <si>
@@ -153,6 +147,27 @@
   </si>
   <si>
     <t xml:space="preserve"> i</t>
+  </si>
+  <si>
+    <t>Player Drop Bomb Ability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player Health Bar </t>
+  </si>
+  <si>
+    <t>Game Level Timer and Bar</t>
+  </si>
+  <si>
+    <t>Game Entry GUI</t>
+  </si>
+  <si>
+    <t>Player  Bomb Drop Limitiatiions by Timer</t>
+  </si>
+  <si>
+    <t>Game Over Animations</t>
+  </si>
+  <si>
+    <t>Special Door Dev</t>
   </si>
 </sst>
 </file>
@@ -240,7 +255,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,12 +289,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9EF8FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -630,8 +639,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+    <xf numFmtId="167" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -657,8 +666,8 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1108,7 +1117,7 @@
   <dimension ref="A1:DX47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:I29"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16"/>
@@ -1723,7 +1732,7 @@
         <f t="shared" si="1"/>
         <v>45767</v>
       </c>
-      <c r="CE4" s="43">
+      <c r="CE4" s="34">
         <f t="shared" si="1"/>
         <v>45768</v>
       </c>
@@ -2558,7 +2567,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>16</v>
@@ -5564,7 +5573,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>16</v>
@@ -5927,7 +5936,7 @@
         <v/>
       </c>
       <c r="CR13" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="CS13" s="7" t="str">
         <f t="shared" si="15"/>
@@ -7066,26 +7075,26 @@
         <v>11</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="30">
-        <v>45734</v>
+        <v>45737</v>
       </c>
       <c r="F16" s="30">
-        <v>45741</v>
+        <v>45744</v>
       </c>
       <c r="G16" s="27">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I16" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="7" t="str">
@@ -7270,7 +7279,7 @@
       </c>
       <c r="BD16" s="7" t="str">
         <f t="shared" si="17"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BE16" s="7" t="str">
         <f t="shared" si="17"/>
@@ -7282,7 +7291,7 @@
       </c>
       <c r="BG16" s="7" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BH16" s="7" t="str">
         <f t="shared" si="18"/>
@@ -7567,7 +7576,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>19</v>
@@ -7583,10 +7592,10 @@
         <v>6</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I17" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="7" t="str">
@@ -8068,7 +8077,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>16</v>
@@ -8569,7 +8578,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>19</v>
@@ -9070,7 +9079,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="31" t="s">
         <v>16</v>
@@ -9086,10 +9095,10 @@
         <v>6</v>
       </c>
       <c r="H20" s="31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I20" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="7" t="str">
@@ -9570,27 +9579,27 @@
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="C21" s="34" t="s">
-        <v>30</v>
+      <c r="C21" s="43" t="s">
+        <v>29</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E21" s="30">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="F21" s="30">
-        <v>45740</v>
+        <v>45743</v>
       </c>
       <c r="G21" s="27">
-        <f t="shared" ref="G21:G29" si="26">IF(F21="","",NETWORKDAYS(E21,F21))</f>
+        <f t="shared" ref="G21:G38" si="26">IF(F21="","",NETWORKDAYS(E21,F21))</f>
         <v>1</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I21" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="7" t="str">
@@ -9771,19 +9780,19 @@
       </c>
       <c r="BC21" s="7" t="str">
         <f>IF(BC$4=$F21,"u","")</f>
+        <v/>
+      </c>
+      <c r="BD21" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BE21" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BF21" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>u</v>
-      </c>
-      <c r="BD21" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BE21" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BF21" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
       </c>
       <c r="BG21" s="7" t="str">
         <f t="shared" si="21"/>
@@ -10072,7 +10081,7 @@
         <v>17</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="31" t="s">
         <v>16</v>
@@ -10088,10 +10097,10 @@
         <v>5</v>
       </c>
       <c r="H22" s="31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I22" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="7" t="str">
@@ -10573,26 +10582,26 @@
         <v>18</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="30">
-        <v>45737</v>
+        <v>45742</v>
       </c>
       <c r="F23" s="30">
-        <v>45744</v>
+        <v>45748</v>
       </c>
       <c r="G23" s="27">
         <f t="shared" si="26"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H23" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I23" s="32">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="7" t="str">
@@ -10789,23 +10798,23 @@
       </c>
       <c r="BG23" s="7" t="str">
         <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BH23" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BI23" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BJ23" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v/>
+      </c>
+      <c r="BK23" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>u</v>
-      </c>
-      <c r="BH23" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BI23" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BJ23" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
-      </c>
-      <c r="BK23" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v/>
       </c>
       <c r="BL23" s="7" t="str">
         <f t="shared" si="21"/>
@@ -11074,10 +11083,10 @@
         <v>19</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E24" s="30">
         <v>45737</v>
@@ -11090,10 +11099,10 @@
         <v>6</v>
       </c>
       <c r="H24" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I24" s="32">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="7" t="str">
@@ -11575,7 +11584,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D25" s="31" t="s">
         <v>19</v>
@@ -11591,10 +11600,10 @@
         <v>6</v>
       </c>
       <c r="H25" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I25" s="32">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="7" t="str">
@@ -12075,25 +12084,27 @@
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="C26" s="24"/>
+      <c r="C26" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="D26" s="31" t="s">
         <v>19</v>
       </c>
       <c r="E26" s="30">
-        <v>45717</v>
+        <v>45744</v>
       </c>
       <c r="F26" s="30">
-        <v>45762</v>
+        <v>45751</v>
       </c>
       <c r="G26" s="27">
         <f t="shared" si="26"/>
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I26" s="32">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="7" t="str">
@@ -12318,7 +12329,7 @@
       </c>
       <c r="BN26" s="7" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BO26" s="7" t="str">
         <f t="shared" si="28"/>
@@ -12362,7 +12373,7 @@
       </c>
       <c r="BY26" s="7" t="str">
         <f t="shared" si="29"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ26" s="7" t="str">
         <f t="shared" si="29"/>
@@ -12574,19 +12585,21 @@
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="C27" s="24"/>
+      <c r="C27" s="24" t="s">
+        <v>39</v>
+      </c>
       <c r="D27" s="31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E27" s="30">
-        <v>45717</v>
+        <v>45744</v>
       </c>
       <c r="F27" s="30">
-        <v>45762</v>
+        <v>45751</v>
       </c>
       <c r="G27" s="27">
         <f t="shared" si="26"/>
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="H27" s="31" t="s">
         <v>12</v>
@@ -12817,7 +12830,7 @@
       </c>
       <c r="BN27" s="7" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BO27" s="7" t="str">
         <f t="shared" si="28"/>
@@ -12861,7 +12874,7 @@
       </c>
       <c r="BY27" s="7" t="str">
         <f t="shared" si="29"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ27" s="7" t="str">
         <f t="shared" si="29"/>
@@ -13073,19 +13086,21 @@
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="C28" s="24"/>
+      <c r="C28" s="24" t="s">
+        <v>40</v>
+      </c>
       <c r="D28" s="31" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E28" s="30">
-        <v>45717</v>
+        <v>45744</v>
       </c>
       <c r="F28" s="30">
-        <v>45762</v>
+        <v>45751</v>
       </c>
       <c r="G28" s="27">
         <f t="shared" si="26"/>
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="H28" s="31" t="s">
         <v>12</v>
@@ -13316,7 +13331,7 @@
       </c>
       <c r="BN28" s="7" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BO28" s="7" t="str">
         <f t="shared" si="28"/>
@@ -13360,7 +13375,7 @@
       </c>
       <c r="BY28" s="7" t="str">
         <f t="shared" si="29"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ28" s="7" t="str">
         <f t="shared" si="29"/>
@@ -13572,19 +13587,21 @@
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="C29" s="24"/>
+      <c r="C29" s="24" t="s">
+        <v>41</v>
+      </c>
       <c r="D29" s="31" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E29" s="30">
-        <v>45717</v>
+        <v>45751</v>
       </c>
       <c r="F29" s="30">
-        <v>45762</v>
+        <v>45758</v>
       </c>
       <c r="G29" s="27">
         <f t="shared" si="26"/>
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="H29" s="31" t="s">
         <v>12</v>
@@ -13843,7 +13860,7 @@
       </c>
       <c r="BU29" s="7" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BV29" s="7" t="str">
         <f t="shared" si="28"/>
@@ -13859,7 +13876,7 @@
       </c>
       <c r="BY29" s="7" t="str">
         <f t="shared" si="29"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ29" s="7" t="str">
         <f t="shared" si="29"/>
@@ -14071,13 +14088,28 @@
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="32"/>
+      <c r="C30" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="30">
+        <v>45751</v>
+      </c>
+      <c r="F30" s="30">
+        <v>45758</v>
+      </c>
+      <c r="G30" s="27">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="32">
+        <v>0</v>
+      </c>
       <c r="J30" s="3"/>
       <c r="K30" s="7" t="str">
         <f t="shared" si="27"/>
@@ -14329,7 +14361,7 @@
       </c>
       <c r="BU30" s="7" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BV30" s="7" t="str">
         <f t="shared" si="28"/>
@@ -14559,11 +14591,22 @@
       </c>
       <c r="C31" s="24"/>
       <c r="D31" s="31"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="32"/>
+      <c r="E31" s="30">
+        <v>45753</v>
+      </c>
+      <c r="F31" s="30">
+        <v>45760</v>
+      </c>
+      <c r="G31" s="27">
+        <f t="shared" si="26"/>
+        <v>5</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="32">
+        <v>0</v>
+      </c>
       <c r="J31" s="3"/>
       <c r="K31" s="7" t="str">
         <f t="shared" si="27"/>
@@ -14823,7 +14866,7 @@
       </c>
       <c r="BW31" s="7" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BX31" s="7" t="str">
         <f t="shared" si="29"/>
@@ -15045,11 +15088,22 @@
       </c>
       <c r="C32" s="24"/>
       <c r="D32" s="31"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="32"/>
+      <c r="E32" s="30">
+        <v>45754</v>
+      </c>
+      <c r="F32" s="30">
+        <v>45761</v>
+      </c>
+      <c r="G32" s="27">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="32">
+        <v>0</v>
+      </c>
       <c r="J32" s="3"/>
       <c r="K32" s="7" t="str">
         <f t="shared" si="27"/>
@@ -15313,7 +15367,7 @@
       </c>
       <c r="BX32" s="7" t="str">
         <f t="shared" si="29"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BY32" s="7" t="str">
         <f t="shared" si="29"/>
@@ -15531,11 +15585,22 @@
       </c>
       <c r="C33" s="24"/>
       <c r="D33" s="31"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="32"/>
+      <c r="E33" s="30">
+        <v>45755</v>
+      </c>
+      <c r="F33" s="30">
+        <v>45762</v>
+      </c>
+      <c r="G33" s="27">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" s="32">
+        <v>0</v>
+      </c>
       <c r="J33" s="3"/>
       <c r="K33" s="7" t="str">
         <f t="shared" ref="K33:Z38" si="35">IF(K$4=$F33,"u","")</f>
@@ -15803,7 +15868,7 @@
       </c>
       <c r="BY33" s="7" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BZ33" s="7" t="str">
         <f t="shared" si="39"/>
@@ -16017,11 +16082,22 @@
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="31"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="32"/>
+      <c r="E34" s="30">
+        <v>45756</v>
+      </c>
+      <c r="F34" s="30">
+        <v>45763</v>
+      </c>
+      <c r="G34" s="27">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="H34" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="32">
+        <v>0</v>
+      </c>
       <c r="J34" s="3"/>
       <c r="K34" s="7" t="str">
         <f t="shared" si="35"/>
@@ -16293,7 +16369,7 @@
       </c>
       <c r="BZ34" s="7" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="CA34" s="7" t="str">
         <f t="shared" si="39"/>
@@ -16503,11 +16579,22 @@
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="31"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="32"/>
+      <c r="E35" s="30">
+        <v>45757</v>
+      </c>
+      <c r="F35" s="30">
+        <v>45764</v>
+      </c>
+      <c r="G35" s="27">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="32">
+        <v>0</v>
+      </c>
       <c r="J35" s="3"/>
       <c r="K35" s="7" t="str">
         <f t="shared" si="35"/>
@@ -16783,7 +16870,7 @@
       </c>
       <c r="CA35" s="7" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="CB35" s="7" t="str">
         <f t="shared" si="39"/>
@@ -16989,11 +17076,22 @@
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="31"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="32"/>
+      <c r="E36" s="30">
+        <v>45758</v>
+      </c>
+      <c r="F36" s="30">
+        <v>45765</v>
+      </c>
+      <c r="G36" s="27">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I36" s="32">
+        <v>0</v>
+      </c>
       <c r="J36" s="3"/>
       <c r="K36" s="7" t="str">
         <f t="shared" si="35"/>
@@ -17273,7 +17371,7 @@
       </c>
       <c r="CB36" s="7" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="CC36" s="7" t="str">
         <f t="shared" si="39"/>
@@ -17475,11 +17573,22 @@
       </c>
       <c r="C37" s="24"/>
       <c r="D37" s="31"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="32"/>
+      <c r="E37" s="30">
+        <v>45759</v>
+      </c>
+      <c r="F37" s="30">
+        <v>45766</v>
+      </c>
+      <c r="G37" s="27">
+        <f t="shared" si="26"/>
+        <v>5</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I37" s="32">
+        <v>0</v>
+      </c>
       <c r="J37" s="3"/>
       <c r="K37" s="7" t="str">
         <f t="shared" si="35"/>
@@ -17763,7 +17872,7 @@
       </c>
       <c r="CC37" s="7" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="CD37" s="7" t="str">
         <f t="shared" si="39"/>
@@ -17961,11 +18070,22 @@
       </c>
       <c r="C38" s="24"/>
       <c r="D38" s="31"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="32"/>
+      <c r="E38" s="30">
+        <v>45760</v>
+      </c>
+      <c r="F38" s="30">
+        <v>45767</v>
+      </c>
+      <c r="G38" s="27">
+        <f t="shared" si="26"/>
+        <v>5</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="32">
+        <v>0</v>
+      </c>
       <c r="J38" s="3"/>
       <c r="K38" s="7" t="str">
         <f t="shared" si="35"/>
@@ -18253,7 +18373,7 @@
       </c>
       <c r="CD38" s="7" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="CE38" s="7" t="str">
         <f t="shared" si="39"/>

</xml_diff>

<commit_message>
edited the giannt chart
</commit_message>
<xml_diff>
--- a/docs/GantChart_Azelele_MGuz.xlsx
+++ b/docs/GantChart_Azelele_MGuz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muratguzelocak/Documents/Projects/FreeBomber/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andri\FinalProject\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B113452A-B5B2-9844-8A9D-52D42346618B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84709399-8352-401D-BC4B-42103478B94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -180,7 +180,7 @@
     <numFmt numFmtId="166" formatCode="mmm\-d\-yy"/>
     <numFmt numFmtId="167" formatCode="mmm\-d"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -556,7 +556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
@@ -665,9 +665,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1116,11 +1113,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF3DB2-1A6B-144B-8344-5E254C7EE240}">
   <dimension ref="A1:DX47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C9" zoomScale="44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
@@ -1145,8 +1142,8 @@
     <col min="77" max="77" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:128" ht="54" customHeight="1" thickBot="1"/>
-    <row r="2" spans="1:128" ht="25" thickBot="1">
+    <row r="1" spans="1:128" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:128" ht="24" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -1281,7 +1278,7 @@
       <c r="DW2" s="38"/>
       <c r="DX2" s="39"/>
     </row>
-    <row r="3" spans="1:128" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1">
+    <row r="3" spans="1:128" s="2" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3"/>
       <c r="B3" s="15"/>
       <c r="C3" s="33" t="s">
@@ -1427,7 +1424,7 @@
       <c r="DW3" s="35"/>
       <c r="DX3" s="36"/>
     </row>
-    <row r="4" spans="1:128" s="1" customFormat="1" ht="41" customHeight="1">
+    <row r="4" spans="1:128" s="1" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4"/>
       <c r="B4" s="18"/>
       <c r="C4" s="19" t="s">
@@ -1917,7 +1914,7 @@
         <v>45813</v>
       </c>
     </row>
-    <row r="5" spans="1:128" ht="23">
+    <row r="5" spans="1:128" ht="25.5" x14ac:dyDescent="0.4">
       <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
@@ -2062,7 +2059,7 @@
       <c r="DW5" s="4"/>
       <c r="DX5" s="11"/>
     </row>
-    <row r="6" spans="1:128" ht="27" customHeight="1">
+    <row r="6" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="23">
         <v>1</v>
       </c>
@@ -2561,7 +2558,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:128" ht="27" customHeight="1">
+    <row r="7" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="23">
         <f>B6+1</f>
         <v>2</v>
@@ -3062,7 +3059,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:128" ht="27" customHeight="1">
+    <row r="8" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" s="23">
         <f t="shared" ref="B8:B38" si="6">B7+1</f>
         <v>3</v>
@@ -3563,7 +3560,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:128" ht="27" customHeight="1">
+    <row r="9" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B9" s="23">
         <f t="shared" si="6"/>
         <v>4</v>
@@ -4064,7 +4061,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:128" ht="27" customHeight="1">
+    <row r="10" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B10" s="23">
         <f t="shared" si="6"/>
         <v>5</v>
@@ -4565,7 +4562,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:128" ht="27" customHeight="1">
+    <row r="11" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="23">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -5066,7 +5063,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:128" ht="27" customHeight="1">
+    <row r="12" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B12" s="23">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -5567,7 +5564,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:128" ht="27" customHeight="1">
+    <row r="13" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B13" s="23">
         <f t="shared" si="6"/>
         <v>8</v>
@@ -6067,7 +6064,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:128" ht="27" customHeight="1">
+    <row r="14" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B14" s="23">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -6568,7 +6565,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:128" ht="27" customHeight="1">
+    <row r="15" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B15" s="23">
         <f t="shared" si="6"/>
         <v>10</v>
@@ -7069,7 +7066,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:128" ht="27" customHeight="1">
+    <row r="16" spans="1:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B16" s="23">
         <f t="shared" si="6"/>
         <v>11</v>
@@ -7570,7 +7567,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:128" ht="27" customHeight="1">
+    <row r="17" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="23">
         <f t="shared" si="6"/>
         <v>12</v>
@@ -8071,7 +8068,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:128" ht="27" customHeight="1">
+    <row r="18" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="23">
         <f t="shared" si="6"/>
         <v>13</v>
@@ -8572,7 +8569,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:128" ht="27" customHeight="1">
+    <row r="19" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="23">
         <f t="shared" si="6"/>
         <v>14</v>
@@ -9073,7 +9070,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:128" ht="27" customHeight="1">
+    <row r="20" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="23">
         <f t="shared" si="6"/>
         <v>15</v>
@@ -9574,12 +9571,12 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:128" ht="27" customHeight="1">
+    <row r="21" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="23">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="24" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="31" t="s">
@@ -10075,7 +10072,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:128" ht="27" customHeight="1">
+    <row r="22" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B22" s="23">
         <f t="shared" si="6"/>
         <v>17</v>
@@ -10576,7 +10573,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:128" ht="27" customHeight="1">
+    <row r="23" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B23" s="23">
         <f t="shared" si="6"/>
         <v>18</v>
@@ -11077,7 +11074,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:128" ht="27" customHeight="1">
+    <row r="24" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="23">
         <f t="shared" si="6"/>
         <v>19</v>
@@ -11102,7 +11099,7 @@
         <v>13</v>
       </c>
       <c r="I24" s="32">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="7" t="str">
@@ -11578,7 +11575,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:128" ht="27" customHeight="1">
+    <row r="25" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B25" s="23">
         <f t="shared" si="6"/>
         <v>20</v>
@@ -12079,7 +12076,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:128" ht="27" customHeight="1">
+    <row r="26" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B26" s="23">
         <f t="shared" si="6"/>
         <v>21</v>
@@ -12580,7 +12577,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:128" ht="27" customHeight="1">
+    <row r="27" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B27" s="23">
         <f t="shared" si="6"/>
         <v>22</v>
@@ -13081,7 +13078,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:128" ht="27" customHeight="1">
+    <row r="28" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B28" s="23">
         <f t="shared" si="6"/>
         <v>23</v>
@@ -13582,7 +13579,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:128" ht="27" customHeight="1">
+    <row r="29" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B29" s="23">
         <f t="shared" si="6"/>
         <v>24</v>
@@ -14083,7 +14080,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="2:128" ht="27" customHeight="1">
+    <row r="30" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B30" s="23">
         <f t="shared" si="6"/>
         <v>25</v>
@@ -14584,7 +14581,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="2:128" ht="27" customHeight="1">
+    <row r="31" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B31" s="23">
         <f t="shared" si="6"/>
         <v>26</v>
@@ -15081,7 +15078,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:128" ht="27" customHeight="1">
+    <row r="32" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B32" s="23">
         <f t="shared" si="6"/>
         <v>27</v>
@@ -15578,7 +15575,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:128" ht="27" customHeight="1">
+    <row r="33" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="23">
         <f t="shared" si="6"/>
         <v>28</v>
@@ -16075,7 +16072,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:128" ht="27" customHeight="1">
+    <row r="34" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B34" s="23">
         <f t="shared" si="6"/>
         <v>29</v>
@@ -16572,7 +16569,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:128" ht="27" customHeight="1">
+    <row r="35" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B35" s="23">
         <f t="shared" si="6"/>
         <v>30</v>
@@ -17069,7 +17066,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:128" ht="27" customHeight="1">
+    <row r="36" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" s="23">
         <f t="shared" si="6"/>
         <v>31</v>
@@ -17566,7 +17563,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:128" ht="27" customHeight="1">
+    <row r="37" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="23">
         <f t="shared" si="6"/>
         <v>32</v>
@@ -18063,7 +18060,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:128" ht="27" customHeight="1">
+    <row r="38" spans="2:128" ht="27" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B38" s="23">
         <f t="shared" si="6"/>
         <v>33</v>
@@ -18560,28 +18557,28 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:128" ht="17" thickBot="1"/>
-    <row r="43" spans="2:128" ht="17" thickBot="1">
+    <row r="42" spans="2:128" ht="16.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="43" spans="2:128" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C43" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="2:128">
+    <row r="44" spans="2:128" x14ac:dyDescent="0.4">
       <c r="C44" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="2:128">
+    <row r="45" spans="2:128" x14ac:dyDescent="0.4">
       <c r="C45" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="2:128">
+    <row r="46" spans="2:128" x14ac:dyDescent="0.4">
       <c r="C46" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="2:128" ht="17" thickBot="1">
+    <row r="47" spans="2:128" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C47" s="13" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
updated the GantChart for the April 9
</commit_message>
<xml_diff>
--- a/docs/GantChart_Azelele_MGuz.xlsx
+++ b/docs/GantChart_Azelele_MGuz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muratguzelocak/Documents/Projects/FreeBomber/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681472DF-5775-4F41-8F20-8AAFB9922065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2F5C7D-9FC6-F644-956B-97D8484FD7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="50">
   <si>
     <t>Project Start Date:</t>
   </si>
@@ -168,6 +168,24 @@
   </si>
   <si>
     <t>Special Door Dev</t>
+  </si>
+  <si>
+    <t>Game Scoreboard</t>
+  </si>
+  <si>
+    <t>Intro Game Manual</t>
+  </si>
+  <si>
+    <t>Bomb Destruction Tile Shape Fix</t>
+  </si>
+  <si>
+    <t>Game Score Count Animation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding Game Points </t>
+  </si>
+  <si>
+    <t>Freaking Javadoc</t>
   </si>
 </sst>
 </file>
@@ -1113,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF3DB2-1A6B-144B-8344-5E254C7EE240}">
   <dimension ref="A1:DX47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AJ48" sqref="AJ48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16"/>
@@ -3084,7 +3102,7 @@
         <v>13</v>
       </c>
       <c r="I8" s="32">
-        <v>0.65</v>
+        <v>0.87</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="7" t="str">
@@ -4086,7 +4104,7 @@
         <v>13</v>
       </c>
       <c r="I10" s="32">
-        <v>0.8</v>
+        <v>0.99</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="7" t="str">
@@ -12098,10 +12116,10 @@
         <v>6</v>
       </c>
       <c r="H26" s="31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I26" s="32">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="7" t="str">
@@ -12602,7 +12620,7 @@
         <v>13</v>
       </c>
       <c r="I27" s="32">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="7" t="str">
@@ -13103,7 +13121,7 @@
         <v>13</v>
       </c>
       <c r="I28" s="32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="7" t="str">
@@ -13601,10 +13619,10 @@
         <v>6</v>
       </c>
       <c r="H29" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I29" s="32">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="7" t="str">
@@ -14102,10 +14120,10 @@
         <v>6</v>
       </c>
       <c r="H30" s="31" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I30" s="32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="7" t="str">
@@ -14586,23 +14604,27 @@
         <f t="shared" si="6"/>
         <v>26</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="31"/>
+      <c r="C31" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>16</v>
+      </c>
       <c r="E31" s="30">
-        <v>45753</v>
+        <v>45751</v>
       </c>
       <c r="F31" s="30">
-        <v>45760</v>
+        <v>45758</v>
       </c>
       <c r="G31" s="27">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I31" s="32">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="7" t="str">
@@ -14855,7 +14877,7 @@
       </c>
       <c r="BU31" s="7" t="str">
         <f t="shared" si="28"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BV31" s="7" t="str">
         <f t="shared" si="28"/>
@@ -14863,7 +14885,7 @@
       </c>
       <c r="BW31" s="7" t="str">
         <f t="shared" si="29"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BX31" s="7" t="str">
         <f t="shared" si="29"/>
@@ -15083,13 +15105,17 @@
         <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="31"/>
+      <c r="C32" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" s="31" t="s">
+        <v>19</v>
+      </c>
       <c r="E32" s="30">
-        <v>45754</v>
+        <v>45758</v>
       </c>
       <c r="F32" s="30">
-        <v>45761</v>
+        <v>45765</v>
       </c>
       <c r="G32" s="27">
         <f t="shared" si="26"/>
@@ -15364,23 +15390,23 @@
       </c>
       <c r="BX32" s="7" t="str">
         <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="BY32" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="BZ32" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="CA32" s="7" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="CB32" s="7" t="str">
+        <f t="shared" si="29"/>
         <v>u</v>
-      </c>
-      <c r="BY32" s="7" t="str">
-        <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="BZ32" s="7" t="str">
-        <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="CA32" s="7" t="str">
-        <f t="shared" si="29"/>
-        <v/>
-      </c>
-      <c r="CB32" s="7" t="str">
-        <f t="shared" si="29"/>
-        <v/>
       </c>
       <c r="CC32" s="7" t="str">
         <f t="shared" si="29"/>
@@ -15580,13 +15606,17 @@
         <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="31"/>
+      <c r="C33" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>16</v>
+      </c>
       <c r="E33" s="30">
-        <v>45755</v>
+        <v>45758</v>
       </c>
       <c r="F33" s="30">
-        <v>45762</v>
+        <v>45765</v>
       </c>
       <c r="G33" s="27">
         <f t="shared" si="26"/>
@@ -15865,7 +15895,7 @@
       </c>
       <c r="BY33" s="7" t="str">
         <f t="shared" si="39"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="BZ33" s="7" t="str">
         <f t="shared" si="39"/>
@@ -15877,7 +15907,7 @@
       </c>
       <c r="CB33" s="7" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="CC33" s="7" t="str">
         <f t="shared" si="39"/>
@@ -16077,13 +16107,17 @@
         <f t="shared" si="6"/>
         <v>29</v>
       </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="31"/>
+      <c r="C34" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="31" t="s">
+        <v>19</v>
+      </c>
       <c r="E34" s="30">
-        <v>45756</v>
+        <v>45758</v>
       </c>
       <c r="F34" s="30">
-        <v>45763</v>
+        <v>45765</v>
       </c>
       <c r="G34" s="27">
         <f t="shared" si="26"/>
@@ -16366,7 +16400,7 @@
       </c>
       <c r="BZ34" s="7" t="str">
         <f t="shared" si="39"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="CA34" s="7" t="str">
         <f t="shared" si="39"/>
@@ -16374,7 +16408,7 @@
       </c>
       <c r="CB34" s="7" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="CC34" s="7" t="str">
         <f t="shared" si="39"/>
@@ -16574,17 +16608,21 @@
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="31"/>
+      <c r="C35" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>16</v>
+      </c>
       <c r="E35" s="30">
-        <v>45757</v>
+        <v>45758</v>
       </c>
       <c r="F35" s="30">
-        <v>45764</v>
+        <v>45763</v>
       </c>
       <c r="G35" s="27">
         <f t="shared" si="26"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H35" s="31" t="s">
         <v>12</v>
@@ -16863,11 +16901,11 @@
       </c>
       <c r="BZ35" s="7" t="str">
         <f t="shared" si="39"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="CA35" s="7" t="str">
         <f t="shared" si="39"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="CB35" s="7" t="str">
         <f t="shared" si="39"/>
@@ -17071,23 +17109,27 @@
         <f t="shared" si="6"/>
         <v>31</v>
       </c>
-      <c r="C36" s="24"/>
-      <c r="D36" s="31"/>
+      <c r="C36" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>26</v>
+      </c>
       <c r="E36" s="30">
+        <v>45756</v>
+      </c>
+      <c r="F36" s="30">
         <v>45758</v>
-      </c>
-      <c r="F36" s="30">
-        <v>45765</v>
       </c>
       <c r="G36" s="27">
         <f t="shared" si="26"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H36" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I36" s="32">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="7" t="str">
@@ -17340,7 +17382,7 @@
       </c>
       <c r="BU36" s="7" t="str">
         <f t="shared" si="38"/>
-        <v/>
+        <v>u</v>
       </c>
       <c r="BV36" s="7" t="str">
         <f t="shared" si="38"/>
@@ -17368,7 +17410,7 @@
       </c>
       <c r="CB36" s="7" t="str">
         <f t="shared" si="39"/>
-        <v>u</v>
+        <v/>
       </c>
       <c r="CC36" s="7" t="str">
         <f t="shared" si="39"/>

</xml_diff>

<commit_message>
updated the Bomb animation and GnatChart and added game manual
</commit_message>
<xml_diff>
--- a/docs/GantChart_Azelele_MGuz.xlsx
+++ b/docs/GantChart_Azelele_MGuz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muratguzelocak/Documents/Projects/FreeBomber/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFF27A9-2C5A-2748-AAD9-41CE40F53F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDBE0E4-68C2-094A-AD9D-9637857EDAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="25700" xr2:uid="{22AD7532-D458-134A-A1AE-ABDB718998AB}"/>
   </bookViews>
@@ -1131,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFFF3DB2-1A6B-144B-8344-5E254C7EE240}">
   <dimension ref="A1:DX47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16"/>
@@ -14621,10 +14621,10 @@
         <v>6</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I31" s="32">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="7" t="str">
@@ -15610,7 +15610,7 @@
         <v>45</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E33" s="30">
         <v>45758</v>
@@ -15623,10 +15623,10 @@
         <v>6</v>
       </c>
       <c r="H33" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I33" s="32">
-        <v>0</v>
+        <v>0.51</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="7" t="str">
@@ -16124,10 +16124,10 @@
         <v>6</v>
       </c>
       <c r="H34" s="31" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I34" s="32">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="7" t="str">
@@ -16625,7 +16625,7 @@
         <v>4</v>
       </c>
       <c r="H35" s="31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I35" s="32">
         <v>0</v>

</xml_diff>